<commit_message>
added more dummy records instead of relying on existing records in local database
</commit_message>
<xml_diff>
--- a/packages/meditrak-server/src/tests/testData/surveyResponses/importResponsesFromMultipleSurveys.xlsx
+++ b/packages/meditrak-server/src/tests/testData/surveyResponses/importResponsesFromMultipleSurveys.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Projects\tupaia\packages\meditrak-server\src\tests\testData\importSurveyResponses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Projects\tupaia\packages\meditrak-server\src\tests\testData\surveyResponses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EB2E69-DE3F-48D8-AF00-B1DBE2B7C81C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F19F11-818A-4EDD-8D42-4256641302E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{374AE92A-F87C-41BB-B830-F4B1DDD546AE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{374AE92A-F87C-41BB-B830-F4B1DDD546AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Clinic Data..." sheetId="1" r:id="rId1"/>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69510686-D67C-43FC-80AD-EA2A52E56C83}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="A1:H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,7 +694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5154EAE5-644C-4917-BB4B-509B434AFDD8}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1026: Fixed failed unit tests
</commit_message>
<xml_diff>
--- a/packages/meditrak-server/src/tests/testData/surveyResponses/importResponsesFromMultipleSurveys.xlsx
+++ b/packages/meditrak-server/src/tests/testData/surveyResponses/importResponsesFromMultipleSurveys.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\Projects\tupaia\packages\meditrak-server\src\tests\testData\surveyResponses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F19F11-818A-4EDD-8D42-4256641302E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DADFC079-06F8-42A2-9F82-ED9369EEDD37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{374AE92A-F87C-41BB-B830-F4B1DDD546AE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{374AE92A-F87C-41BB-B830-F4B1DDD546AE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Basic Clinic Data..." sheetId="1" r:id="rId1"/>
-    <sheet name="Facility Fundamentals" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Import Survey Response 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Import Survey Response 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -523,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69510686-D67C-43FC-80AD-EA2A52E56C83}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -694,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5154EAE5-644C-4917-BB4B-509B434AFDD8}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>